<commit_message>
Fixed NaN exclusion bug
There was some discrepancy between at what point the NaN behavior data was excluded. Changed it so if one behavior event is  a NaN it just gets excluded instead of making the whole cell P-val NaN.
</commit_message>
<xml_diff>
--- a/Paper Rebuttal/Adjustments_12_2019/Data/results_significance_N_all_time.xlsx
+++ b/Paper Rebuttal/Adjustments_12_2019/Data/results_significance_N_all_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lccam\Documents\CU Boulder\Donaldson Lab\Imaging-Paper\Paper Rebuttal\Adjustments_12_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32011002-0178-4F66-BC53-47ACF64C59F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E33B3869-4730-434B-B233-8ED3281808DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{7372B79A-7E64-4C89-8AE7-8575C90F33CA}"/>
   </bookViews>
@@ -563,10 +563,10 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>5.5555555555555552E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>0.22222222222222221</v>
@@ -581,10 +581,10 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>5.5555555555555552E-2</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0.1111111111111111</v>
@@ -681,10 +681,10 @@
         <v>2</v>
       </c>
       <c r="N5">
-        <v>6.5217391304347824E-2</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="O5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -704,10 +704,10 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <v>0.27500000000000002</v>
@@ -722,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6">
         <v>0.1</v>
@@ -763,10 +763,10 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>3.3333333333333333E-2</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>3.3333333333333333E-2</v>
@@ -792,10 +792,10 @@
         <v>56</v>
       </c>
       <c r="D8">
-        <v>5.3571428571428568E-2</v>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>8.9285714285714288E-2</v>
@@ -810,22 +810,22 @@
         <v>9</v>
       </c>
       <c r="J8">
-        <v>8.9285714285714288E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="K8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L8">
-        <v>8.9285714285714288E-2</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N8">
-        <v>0.16071428571428573</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="O8">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -845,16 +845,16 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0.1</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <v>3.3333333333333333E-2</v>
@@ -863,10 +863,10 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>0.13333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="M9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N9">
         <v>0.2</v>
@@ -957,16 +957,16 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>5.8823529411764705E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>0.11764705882352941</v>
+        <v>8.8235294117647065E-2</v>
       </c>
       <c r="O11">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -980,22 +980,22 @@
         <v>38</v>
       </c>
       <c r="D12">
-        <v>2.6315789473684209E-2</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>7.8947368421052627E-2</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>0.15789473684210525</v>
+        <v>0.18421052631578946</v>
       </c>
       <c r="I12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J12">
         <v>2.6315789473684209E-2</v>
@@ -1039,10 +1039,10 @@
         <v>2</v>
       </c>
       <c r="H13">
-        <v>0.10714285714285714</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13">
         <v>7.1428571428571425E-2</v>
@@ -1051,10 +1051,10 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>7.1428571428571425E-2</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13">
         <v>0.10714285714285714</v>
@@ -1098,10 +1098,10 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>8.6956521739130432E-2</v>
@@ -1118,40 +1118,40 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>3.125E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>6.25E-2</v>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15">
-        <v>0.125</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="I15">
         <v>4</v>
       </c>
       <c r="J15">
-        <v>3.125E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15">
-        <v>3.125E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
       <c r="N15">
-        <v>9.375E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="O15">
         <v>3</v>
@@ -1168,10 +1168,10 @@
         <v>31</v>
       </c>
       <c r="D16">
-        <v>3.2258064516129031E-2</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>9.6774193548387094E-2</v>
@@ -1180,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="H16">
-        <v>0.19354838709677419</v>
+        <v>0.22580645161290322</v>
       </c>
       <c r="I16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J16">
         <v>3.2258064516129031E-2</v>
@@ -1262,10 +1262,10 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>0.22222222222222221</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18">
         <v>0.33333333333333331</v>
@@ -1274,10 +1274,10 @@
         <v>6</v>
       </c>
       <c r="H18">
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J18">
         <v>5.5555555555555552E-2</v>
@@ -1309,22 +1309,22 @@
         <v>45</v>
       </c>
       <c r="D19">
-        <v>0.31111111111111112</v>
+        <v>0.28888888888888886</v>
       </c>
       <c r="E19">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>0.35555555555555557</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19">
-        <v>0.46666666666666667</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="I19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J19">
         <v>6.6666666666666666E-2</v>
@@ -1339,10 +1339,10 @@
         <v>4</v>
       </c>
       <c r="N19">
-        <v>0.13333333333333333</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="O19">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1356,10 +1356,10 @@
         <v>50</v>
       </c>
       <c r="D20">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="E20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F20">
         <v>0.28000000000000003</v>
@@ -1374,16 +1374,16 @@
         <v>15</v>
       </c>
       <c r="J20">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="M20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N20">
         <v>0.14000000000000001</v>
@@ -1403,16 +1403,16 @@
         <v>40</v>
       </c>
       <c r="D21">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>0.27500000000000002</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="G21">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H21">
         <v>0.45</v>
@@ -1427,10 +1427,10 @@
         <v>2</v>
       </c>
       <c r="L21">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="M21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N21">
         <v>0.125</v>
@@ -1450,10 +1450,10 @@
         <v>43</v>
       </c>
       <c r="D22">
-        <v>0.11627906976744186</v>
+        <v>9.3023255813953487E-2</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>0.13953488372093023</v>
@@ -1468,10 +1468,10 @@
         <v>7</v>
       </c>
       <c r="J22">
-        <v>9.3023255813953487E-2</v>
+        <v>0.11627906976744186</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L22">
         <v>0.11627906976744186</v>
@@ -1509,16 +1509,16 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>6.6666666666666666E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23">
-        <v>0.13333333333333333</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L23">
         <v>0.17777777777777778</v>
@@ -1620,10 +1620,10 @@
         <v>59</v>
       </c>
       <c r="D26">
-        <v>0.3728813559322034</v>
+        <v>0.32203389830508472</v>
       </c>
       <c r="E26">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F26">
         <v>0.38983050847457629</v>
@@ -1650,10 +1650,10 @@
         <v>21</v>
       </c>
       <c r="N26">
-        <v>0.4576271186440678</v>
+        <v>0.44067796610169491</v>
       </c>
       <c r="O26">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -1696,16 +1696,16 @@
         <v>23</v>
       </c>
       <c r="D28">
-        <v>8.6956521739130432E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>0.17391304347826086</v>
+        <v>0.21739130434782608</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28">
         <v>0.2608695652173913</v>
@@ -1743,10 +1743,10 @@
         <v>35</v>
       </c>
       <c r="D29">
-        <v>0.17142857142857143</v>
+        <v>0.2</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <v>0.22857142857142856</v>
@@ -1755,10 +1755,10 @@
         <v>8</v>
       </c>
       <c r="H29">
-        <v>0.2857142857142857</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="I29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J29">
         <v>2.8571428571428571E-2</v>
@@ -1960,10 +1960,10 @@
         <v>34</v>
       </c>
       <c r="D34">
-        <v>5.8823529411764705E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0.11764705882352941</v>
@@ -1990,10 +1990,10 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>8.8235294117647065E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="O34">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -2060,10 +2060,10 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0.15</v>
@@ -2084,10 +2084,10 @@
         <v>2</v>
       </c>
       <c r="N36">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="O36">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -2131,10 +2131,10 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <v>9.5238095238095233E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="O37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2272,10 +2272,10 @@
         <v>2</v>
       </c>
       <c r="N40">
-        <v>0.10344827586206896</v>
+        <v>0.13793103448275862</v>
       </c>
       <c r="O40">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -2295,34 +2295,34 @@
         <v>4</v>
       </c>
       <c r="F41">
-        <v>0.16666666666666666</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H41">
-        <v>0.19047619047619047</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="I41">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J41">
-        <v>7.1428571428571425E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="K41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L41">
-        <v>0.11904761904761904</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="M41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N41">
-        <v>0.11904761904761904</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="O41">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -2342,10 +2342,10 @@
         <v>4</v>
       </c>
       <c r="F42">
-        <v>8.6956521739130432E-2</v>
+        <v>5.7971014492753624E-2</v>
       </c>
       <c r="G42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H42">
         <v>0.15942028985507245</v>
@@ -2389,16 +2389,16 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>5.4945054945054944E-2</v>
+        <v>6.5934065934065936E-2</v>
       </c>
       <c r="G43">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H43">
-        <v>9.8901098901098897E-2</v>
+        <v>0.10989010989010989</v>
       </c>
       <c r="I43">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J43">
         <v>2.197802197802198E-2</v>
@@ -2413,10 +2413,10 @@
         <v>5</v>
       </c>
       <c r="N43">
-        <v>8.7912087912087919E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="O43">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -2436,10 +2436,10 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>0.16666666666666666</v>
@@ -2530,22 +2530,22 @@
         <v>2</v>
       </c>
       <c r="F46">
-        <v>9.0909090909090912E-2</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H46">
-        <v>0.18181818181818182</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="I46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J46">
-        <v>0.18181818181818182</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="K46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L46">
         <v>0.22727272727272727</v>
@@ -2583,10 +2583,10 @@
         <v>3</v>
       </c>
       <c r="H47">
-        <v>0.16666666666666666</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2642,16 +2642,16 @@
         <v>6</v>
       </c>
       <c r="L48">
-        <v>0.16326530612244897</v>
+        <v>0.18367346938775511</v>
       </c>
       <c r="M48">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N48">
-        <v>0.30612244897959184</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="O48">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -2677,10 +2677,10 @@
         <v>9</v>
       </c>
       <c r="H49">
-        <v>0.21428571428571427</v>
+        <v>0.19642857142857142</v>
       </c>
       <c r="I49">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J49">
         <v>1.7857142857142856E-2</v>
@@ -2689,10 +2689,10 @@
         <v>1</v>
       </c>
       <c r="L49">
-        <v>1.7857142857142856E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="M49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N49">
         <v>8.9285714285714288E-2</v>
@@ -2730,22 +2730,22 @@
         <v>4</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
-        <v>4.2553191489361701E-2</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="M50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N50">
-        <v>8.5106382978723402E-2</v>
+        <v>6.3829787234042548E-2</v>
       </c>
       <c r="O50">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -2759,16 +2759,16 @@
         <v>42</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>4.7619047619047616E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>4.7619047619047616E-2</v>
@@ -2783,10 +2783,10 @@
         <v>2</v>
       </c>
       <c r="L51">
-        <v>0.11904761904761904</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="M51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N51">
         <v>0.16666666666666666</v>
@@ -2812,10 +2812,10 @@
         <v>3</v>
       </c>
       <c r="F52">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H52">
         <v>0.15</v>
@@ -2824,10 +2824,10 @@
         <v>6</v>
       </c>
       <c r="J52">
-        <v>2.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52">
         <v>0.05</v>
@@ -2853,10 +2853,10 @@
         <v>37</v>
       </c>
       <c r="D53">
-        <v>5.4054054054054057E-2</v>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53">
         <v>0.10810810810810811</v>
@@ -2871,10 +2871,10 @@
         <v>8</v>
       </c>
       <c r="J53">
-        <v>2.7027027027027029E-2</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53">
         <v>5.4054054054054057E-2</v>
@@ -2883,10 +2883,10 @@
         <v>2</v>
       </c>
       <c r="N53">
-        <v>8.1081081081081086E-2</v>
+        <v>5.4054054054054057E-2</v>
       </c>
       <c r="O53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -2900,10 +2900,10 @@
         <v>38</v>
       </c>
       <c r="D54">
-        <v>7.8947368421052627E-2</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54">
         <v>0.10526315789473684</v>
@@ -2953,10 +2953,10 @@
         <v>6</v>
       </c>
       <c r="F55">
-        <v>0.20689655172413793</v>
+        <v>0.2413793103448276</v>
       </c>
       <c r="G55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H55">
         <v>0.2413793103448276</v>
@@ -2977,10 +2977,10 @@
         <v>2</v>
       </c>
       <c r="N55">
-        <v>6.8965517241379309E-2</v>
+        <v>0.10344827586206896</v>
       </c>
       <c r="O55">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>